<commit_message>
Atualização automática dos dados: Sat Jan 17 11:42:25 UTC 2026
</commit_message>
<xml_diff>
--- a/dados_dashboard.xlsx
+++ b/dados_dashboard.xlsx
@@ -477,7 +477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,12 +488,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>CUSTO DESENVOLVIMENTO</t>
+          <t>REFUGO REAL (PROCESSO)</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>R$ 68.563,94</t>
+          <t>R$ 236.618,39</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -503,12 +503,12 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>R$ 68.563,94</t>
+          <t>R$ 236.618,39</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>R$ 68.563,94</t>
+          <t>R$ 236.618,39</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -520,76 +520,76 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>EMBALAGENS</t>
+          <t>MATERIA PRIMA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>R$ 47.974,08</t>
+          <t>R$ 234.121,48</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>R$ 52.522,04</t>
+          <t>R$ 0,00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>R$ 100.496,12</t>
+          <t>R$ 234.121,48</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>R$ 160.000,00</t>
+          <t>R$ 1,00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>62,81 %</t>
+          <t>23.412.148,00 %</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DESP. INDUSTRIAL</t>
+          <t>FRETES</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>R$ 40.002,66</t>
+          <t>R$ 179.648,09</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>R$ 100.235,94</t>
+          <t>R$ 0,00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>R$ 140.238,60</t>
+          <t>R$ 179.648,09</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>R$ 470.000,00</t>
+          <t>R$ 376.000,00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>29,84 %</t>
+          <t>47,78 %</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SERVICOS DE QUALIDADE</t>
+          <t>REFUGO MP+CP*</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>R$ 38.449,82</t>
+          <t>R$ 141.770,84</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -599,175 +599,367 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>R$ 38.449,82</t>
+          <t>R$ 141.770,84</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>R$ 45.000,00</t>
+          <t>R$ 285.000,00</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>85,44 %</t>
+          <t>49,74 %</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CUSTO COM DESENVOLVIMENTO</t>
+          <t>MANUTENCAO</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>R$ 8.301,08</t>
+          <t>R$ 121.296,45</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>R$ 0,00</t>
+          <t>R$ 269.190,05</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>R$ 8.301,08</t>
+          <t>R$ 390.486,50</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>R$ 8.301,08</t>
+          <t>R$ 480.000,00</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>100,00 %</t>
+          <t>81,35 %</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>FERRAMENTARIA/MAN FR</t>
+          <t>OLEOS E LUBRIFICANTES</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>R$ 7.268,32</t>
+          <t>R$ 80.508,54</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>R$ 0,00</t>
+          <t>R$ 108.573,04</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>R$ 7.268,32</t>
+          <t>R$ 189.081,58</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>R$ 35.000,00</t>
+          <t>R$ 280.000,00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>20,77 %</t>
+          <t>67,53 %</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MATERIAL QUALIDADE</t>
+          <t>CUSTO DESENVOLVIMENTO</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>R$ 110,37</t>
+          <t>R$ 68.563,94</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>R$ 4.033,80</t>
+          <t>R$ 0,00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>R$ 4.144,17</t>
+          <t>R$ 68.563,94</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>R$ 45.000,00</t>
+          <t>R$ 68.563,94</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>9,21 %</t>
+          <t>100,00 %</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ENERGIA ELETRICA</t>
+          <t>EMBALAGENS</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>R$ 0,00</t>
+          <t>R$ 47.974,08</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>R$ 0,00</t>
+          <t>R$ 52.522,04</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>R$ 0,00</t>
+          <t>R$ 100.496,12</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>R$ 519.000,00</t>
+          <t>R$ 160.000,00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0 %</t>
+          <t>62,81 %</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>DESP. INDUSTRIAL</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>R$ 40.002,66</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>R$ 100.281,50</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>R$ 140.284,16</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>R$ 470.000,00</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>29,85 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>SERVICOS DE QUALIDADE</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>R$ 38.449,82</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>R$ 0,00</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>R$ 38.449,82</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>R$ 45.000,00</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>85,44 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>CUSTO COM DESENVOLVIMENTO</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>R$ 8.301,08</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>R$ 0,00</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>R$ 8.301,08</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>R$ 8.301,08</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>100,00 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>FERRAMENTARIA/MAN FR</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>R$ 7.268,32</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>R$ 0,00</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>R$ 7.268,32</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>R$ 35.000,00</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>20,77 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>MATERIAL QUALIDADE</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>R$ 110,37</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>R$ 4.033,80</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>R$ 4.144,17</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>R$ 45.000,00</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>9,21 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>ENERGIA ELETRICA</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>R$ 0,00</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>R$ 0,00</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>R$ 0,00</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>R$ 519.000,00</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>0 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
           <t>Total Geral</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
+      <c r="B15" t="inlineStr">
         <is>
           <t>R$ 1.767.242,29</t>
         </is>
       </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>R$ 534.554,87</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>R$ 2.301.797,16</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>R$ 534.600,42</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>R$ 2.301.842,71</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
         <is>
           <t>R$ 3.835.922,27</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
+      <c r="F15" t="inlineStr">
         <is>
           <t>60,01 %</t>
         </is>

</xml_diff>

<commit_message>
Atualização automática dos dados: Sat Jan 17 11:54:59 UTC 2026
</commit_message>
<xml_diff>
--- a/dados_dashboard.xlsx
+++ b/dados_dashboard.xlsx
@@ -477,7 +477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F15"/>
+  <dimension ref="A1:F9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,12 +488,12 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>REFUGO REAL (PROCESSO)</t>
+          <t>CUSTO DESENVOLVIMENTO</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>R$ 236.618,39</t>
+          <t>R$ 68.563,94</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
@@ -503,12 +503,12 @@
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>R$ 236.618,39</t>
+          <t>R$ 68.563,94</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>R$ 236.618,39</t>
+          <t>R$ 68.563,94</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
@@ -520,76 +520,76 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>MATERIA PRIMA</t>
+          <t>EMBALAGENS</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>R$ 234.121,48</t>
+          <t>R$ 47.974,08</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>R$ 0,00</t>
+          <t>R$ 52.522,04</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>R$ 234.121,48</t>
+          <t>R$ 100.496,12</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>R$ 1,00</t>
+          <t>R$ 160.000,00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>23.412.148,00 %</t>
+          <t>62,81 %</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>FRETES</t>
+          <t>DESP. INDUSTRIAL</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>R$ 179.648,09</t>
+          <t>R$ 40.002,66</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>R$ 0,00</t>
+          <t>R$ 100.281,50</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>R$ 179.648,09</t>
+          <t>R$ 140.284,16</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>R$ 376.000,00</t>
+          <t>R$ 470.000,00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>47,78 %</t>
+          <t>29,85 %</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>REFUGO MP+CP*</t>
+          <t>SERVICOS DE QUALIDADE</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>R$ 141.770,84</t>
+          <t>R$ 38.449,82</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -599,367 +599,175 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>R$ 141.770,84</t>
+          <t>R$ 38.449,82</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>R$ 285.000,00</t>
+          <t>R$ 45.000,00</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>49,74 %</t>
+          <t>85,44 %</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>MANUTENCAO</t>
+          <t>CUSTO COM DESENVOLVIMENTO</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>R$ 121.296,45</t>
+          <t>R$ 8.301,08</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>R$ 269.190,05</t>
+          <t>R$ 0,00</t>
         </is>
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>R$ 390.486,50</t>
+          <t>R$ 8.301,08</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>R$ 480.000,00</t>
+          <t>R$ 8.301,08</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
         <is>
-          <t>81,35 %</t>
+          <t>100,00 %</t>
         </is>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>OLEOS E LUBRIFICANTES</t>
+          <t>FERRAMENTARIA/MAN FR</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>R$ 80.508,54</t>
+          <t>R$ 7.268,32</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>R$ 108.573,04</t>
+          <t>R$ 0,00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>R$ 189.081,58</t>
+          <t>R$ 7.268,32</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>R$ 280.000,00</t>
+          <t>R$ 35.000,00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>67,53 %</t>
+          <t>20,77 %</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>CUSTO DESENVOLVIMENTO</t>
+          <t>MATERIAL QUALIDADE</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>R$ 68.563,94</t>
+          <t>R$ 110,37</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>R$ 0,00</t>
+          <t>R$ 4.033,80</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>R$ 68.563,94</t>
+          <t>R$ 4.144,17</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>R$ 68.563,94</t>
+          <t>R$ 45.000,00</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>100,00 %</t>
+          <t>9,21 %</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>EMBALAGENS</t>
+          <t>ENERGIA ELETRICA</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>R$ 47.974,08</t>
+          <t>R$ 0,00</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>R$ 52.522,04</t>
+          <t>R$ 0,00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>R$ 100.496,12</t>
+          <t>R$ 0,00</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>R$ 160.000,00</t>
+          <t>R$ 519.000,00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>62,81 %</t>
+          <t>0 %</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>DESP. INDUSTRIAL</t>
+          <t>Total Geral</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>R$ 40.002,66</t>
+          <t>R$ 1.767.242,29</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>R$ 100.281,50</t>
+          <t>R$ 534.600,42</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>R$ 140.284,16</t>
+          <t>R$ 2.301.842,71</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>R$ 470.000,00</t>
+          <t>R$ 3.835.922,27</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
-        <is>
-          <t>29,85 %</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" t="inlineStr">
-        <is>
-          <t>SERVICOS DE QUALIDADE</t>
-        </is>
-      </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>R$ 38.449,82</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>R$ 0,00</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>R$ 38.449,82</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>R$ 45.000,00</t>
-        </is>
-      </c>
-      <c r="F10" t="inlineStr">
-        <is>
-          <t>85,44 %</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" t="inlineStr">
-        <is>
-          <t>CUSTO COM DESENVOLVIMENTO</t>
-        </is>
-      </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>R$ 8.301,08</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>R$ 0,00</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>R$ 8.301,08</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>R$ 8.301,08</t>
-        </is>
-      </c>
-      <c r="F11" t="inlineStr">
-        <is>
-          <t>100,00 %</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" t="inlineStr">
-        <is>
-          <t>FERRAMENTARIA/MAN FR</t>
-        </is>
-      </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>R$ 7.268,32</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>R$ 0,00</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>R$ 7.268,32</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>R$ 35.000,00</t>
-        </is>
-      </c>
-      <c r="F12" t="inlineStr">
-        <is>
-          <t>20,77 %</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" t="inlineStr">
-        <is>
-          <t>MATERIAL QUALIDADE</t>
-        </is>
-      </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>R$ 110,37</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>R$ 4.033,80</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>R$ 4.144,17</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>R$ 45.000,00</t>
-        </is>
-      </c>
-      <c r="F13" t="inlineStr">
-        <is>
-          <t>9,21 %</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" t="inlineStr">
-        <is>
-          <t>ENERGIA ELETRICA</t>
-        </is>
-      </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>R$ 0,00</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>R$ 0,00</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>R$ 0,00</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>R$ 519.000,00</t>
-        </is>
-      </c>
-      <c r="F14" t="inlineStr">
-        <is>
-          <t>0 %</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" t="inlineStr">
-        <is>
-          <t>Total Geral</t>
-        </is>
-      </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>R$ 1.767.242,29</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>R$ 534.600,42</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>R$ 2.301.842,71</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>R$ 3.835.922,27</t>
-        </is>
-      </c>
-      <c r="F15" t="inlineStr">
         <is>
           <t>60,01 %</t>
         </is>

</xml_diff>

<commit_message>
Atualização automática dos dados: Mon Jan 19 09:39:31 UTC 2026
</commit_message>
<xml_diff>
--- a/dados_dashboard.xlsx
+++ b/dados_dashboard.xlsx
@@ -477,7 +477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F9"/>
+  <dimension ref="A1:F18"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -488,108 +488,108 @@
     <row r="1">
       <c r="A1" s="1" t="inlineStr">
         <is>
-          <t>CUSTO DESENVOLVIMENTO</t>
+          <t>DescriÃ§Ã£o da despesa</t>
         </is>
       </c>
       <c r="B1" s="1" t="inlineStr">
         <is>
-          <t>R$ 68.563,94</t>
+          <t>Entrada</t>
         </is>
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>R$ 0,00</t>
+          <t>Consumo</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
         <is>
-          <t>R$ 68.563,94</t>
+          <t>Gasto Total</t>
         </is>
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>R$ 68.563,94</t>
+          <t>Budget MÃªs</t>
         </is>
       </c>
       <c r="F1" s="1" t="inlineStr">
         <is>
-          <t>100,00 %</t>
+          <t>Percentual</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>EMBALAGENS</t>
+          <t>DEVOLUÃÃO</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>R$ 47.974,08</t>
+          <t>R$ 382.437,86</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
         <is>
-          <t>R$ 52.522,04</t>
+          <t>R$ 0,00</t>
         </is>
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>R$ 100.496,12</t>
+          <t>R$ 382.437,86</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>R$ 160.000,00</t>
+          <t>R$ 382.437,86</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>62,81 %</t>
+          <t>100,00 %</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DESP. INDUSTRIAL</t>
+          <t>FERRAMENTAS/ MATRIZARIA</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>R$ 40.002,66</t>
+          <t>R$ 321.941,21</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>R$ 100.281,50</t>
+          <t>R$ 0,00</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>R$ 140.284,16</t>
+          <t>R$ 321.941,21</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>R$ 470.000,00</t>
+          <t>R$ 730.000,00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>29,85 %</t>
+          <t>44,10 %</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>SERVICOS DE QUALIDADE</t>
+          <t>MATERIA PRIMA</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>R$ 38.449,82</t>
+          <t>R$ 286.256,71</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -599,29 +599,29 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>R$ 38.449,82</t>
+          <t>R$ 286.256,71</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>R$ 45.000,00</t>
+          <t>R$ 1,00</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>85,44 %</t>
+          <t>28.625.671,00 %</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>CUSTO COM DESENVOLVIMENTO</t>
+          <t>REFUGO REAL (PROCESSO)</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>R$ 8.301,08</t>
+          <t>R$ 236.618,39</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -631,12 +631,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>R$ 8.301,08</t>
+          <t>R$ 236.618,39</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>R$ 8.301,08</t>
+          <t>R$ 236.618,39</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -648,12 +648,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>FERRAMENTARIA/MAN FR</t>
+          <t>FRETES</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>R$ 7.268,32</t>
+          <t>R$ 185.370,49</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -663,113 +663,401 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>R$ 7.268,32</t>
+          <t>R$ 185.370,49</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>R$ 35.000,00</t>
+          <t>R$ 376.000,00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>20,77 %</t>
+          <t>49,30 %</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MATERIAL QUALIDADE</t>
+          <t>REFUGO MP+CP*</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>R$ 110,37</t>
+          <t>R$ 141.770,66</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>R$ 4.033,80</t>
+          <t>R$ 0,00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>R$ 4.144,17</t>
+          <t>R$ 141.770,66</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>R$ 45.000,00</t>
+          <t>R$ 285.000,00</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>9,21 %</t>
+          <t>49,74 %</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>ENERGIA ELETRICA</t>
+          <t>MANUTENCAO</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>R$ 0,00</t>
+          <t>R$ 125.498,86</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>R$ 0,00</t>
+          <t>R$ 269.255,54</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>R$ 0,00</t>
+          <t>R$ 394.754,40</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>R$ 519.000,00</t>
+          <t>R$ 480.000,00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>0 %</t>
+          <t>82,24 %</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
+          <t>OLEOS E LUBRIFICANTES</t>
+        </is>
+      </c>
+      <c r="B9" t="inlineStr">
+        <is>
+          <t>R$ 82.091,98</t>
+        </is>
+      </c>
+      <c r="C9" t="inlineStr">
+        <is>
+          <t>R$ 108.592,70</t>
+        </is>
+      </c>
+      <c r="D9" t="inlineStr">
+        <is>
+          <t>R$ 190.684,68</t>
+        </is>
+      </c>
+      <c r="E9" t="inlineStr">
+        <is>
+          <t>R$ 280.000,00</t>
+        </is>
+      </c>
+      <c r="F9" t="inlineStr">
+        <is>
+          <t>68,10 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="10">
+      <c r="A10" t="inlineStr">
+        <is>
+          <t>CUSTO DESENVOLVIMENTO</t>
+        </is>
+      </c>
+      <c r="B10" t="inlineStr">
+        <is>
+          <t>R$ 68.563,94</t>
+        </is>
+      </c>
+      <c r="C10" t="inlineStr">
+        <is>
+          <t>R$ 0,00</t>
+        </is>
+      </c>
+      <c r="D10" t="inlineStr">
+        <is>
+          <t>R$ 68.563,94</t>
+        </is>
+      </c>
+      <c r="E10" t="inlineStr">
+        <is>
+          <t>R$ 68.563,94</t>
+        </is>
+      </c>
+      <c r="F10" t="inlineStr">
+        <is>
+          <t>100,00 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="11">
+      <c r="A11" t="inlineStr">
+        <is>
+          <t>DESP. INDUSTRIAL</t>
+        </is>
+      </c>
+      <c r="B11" t="inlineStr">
+        <is>
+          <t>R$ 56.748,18</t>
+        </is>
+      </c>
+      <c r="C11" t="inlineStr">
+        <is>
+          <t>R$ 102.917,80</t>
+        </is>
+      </c>
+      <c r="D11" t="inlineStr">
+        <is>
+          <t>R$ 159.665,98</t>
+        </is>
+      </c>
+      <c r="E11" t="inlineStr">
+        <is>
+          <t>R$ 470.000,00</t>
+        </is>
+      </c>
+      <c r="F11" t="inlineStr">
+        <is>
+          <t>33,97 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" t="inlineStr">
+        <is>
+          <t>EMBALAGENS</t>
+        </is>
+      </c>
+      <c r="B12" t="inlineStr">
+        <is>
+          <t>R$ 47.974,08</t>
+        </is>
+      </c>
+      <c r="C12" t="inlineStr">
+        <is>
+          <t>R$ 52.522,04</t>
+        </is>
+      </c>
+      <c r="D12" t="inlineStr">
+        <is>
+          <t>R$ 100.496,12</t>
+        </is>
+      </c>
+      <c r="E12" t="inlineStr">
+        <is>
+          <t>R$ 160.000,00</t>
+        </is>
+      </c>
+      <c r="F12" t="inlineStr">
+        <is>
+          <t>62,81 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" t="inlineStr">
+        <is>
+          <t>SERVICOS DE QUALIDADE</t>
+        </is>
+      </c>
+      <c r="B13" t="inlineStr">
+        <is>
+          <t>R$ 43.762,33</t>
+        </is>
+      </c>
+      <c r="C13" t="inlineStr">
+        <is>
+          <t>R$ 0,00</t>
+        </is>
+      </c>
+      <c r="D13" t="inlineStr">
+        <is>
+          <t>R$ 43.762,33</t>
+        </is>
+      </c>
+      <c r="E13" t="inlineStr">
+        <is>
+          <t>R$ 45.000,00</t>
+        </is>
+      </c>
+      <c r="F13" t="inlineStr">
+        <is>
+          <t>97,25 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" t="inlineStr">
+        <is>
+          <t>CUSTO COM DESENVOLVIMENTO</t>
+        </is>
+      </c>
+      <c r="B14" t="inlineStr">
+        <is>
+          <t>R$ 8.301,08</t>
+        </is>
+      </c>
+      <c r="C14" t="inlineStr">
+        <is>
+          <t>R$ 0,00</t>
+        </is>
+      </c>
+      <c r="D14" t="inlineStr">
+        <is>
+          <t>R$ 8.301,08</t>
+        </is>
+      </c>
+      <c r="E14" t="inlineStr">
+        <is>
+          <t>R$ 8.301,08</t>
+        </is>
+      </c>
+      <c r="F14" t="inlineStr">
+        <is>
+          <t>100,00 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" t="inlineStr">
+        <is>
+          <t>FERRAMENTARIA/MAN FR</t>
+        </is>
+      </c>
+      <c r="B15" t="inlineStr">
+        <is>
+          <t>R$ 7.268,32</t>
+        </is>
+      </c>
+      <c r="C15" t="inlineStr">
+        <is>
+          <t>R$ 0,00</t>
+        </is>
+      </c>
+      <c r="D15" t="inlineStr">
+        <is>
+          <t>R$ 7.268,32</t>
+        </is>
+      </c>
+      <c r="E15" t="inlineStr">
+        <is>
+          <t>R$ 35.000,00</t>
+        </is>
+      </c>
+      <c r="F15" t="inlineStr">
+        <is>
+          <t>20,77 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" t="inlineStr">
+        <is>
+          <t>MATERIAL QUALIDADE</t>
+        </is>
+      </c>
+      <c r="B16" t="inlineStr">
+        <is>
+          <t>R$ 110,37</t>
+        </is>
+      </c>
+      <c r="C16" t="inlineStr">
+        <is>
+          <t>R$ 4.033,80</t>
+        </is>
+      </c>
+      <c r="D16" t="inlineStr">
+        <is>
+          <t>R$ 4.144,17</t>
+        </is>
+      </c>
+      <c r="E16" t="inlineStr">
+        <is>
+          <t>R$ 45.000,00</t>
+        </is>
+      </c>
+      <c r="F16" t="inlineStr">
+        <is>
+          <t>9,21 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" t="inlineStr">
+        <is>
+          <t>ENERGIA ELETRICA</t>
+        </is>
+      </c>
+      <c r="B17" t="inlineStr">
+        <is>
+          <t>R$ 0,00</t>
+        </is>
+      </c>
+      <c r="C17" t="inlineStr">
+        <is>
+          <t>R$ 0,00</t>
+        </is>
+      </c>
+      <c r="D17" t="inlineStr">
+        <is>
+          <t>R$ 0,00</t>
+        </is>
+      </c>
+      <c r="E17" t="inlineStr">
+        <is>
+          <t>R$ 519.000,00</t>
+        </is>
+      </c>
+      <c r="F17" t="inlineStr">
+        <is>
+          <t>0 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" t="inlineStr">
+        <is>
           <t>Total Geral</t>
         </is>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>R$ 1.767.242,29</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>R$ 534.600,42</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>R$ 2.301.842,71</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>R$ 1.852.943,80</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>R$ 537.321,89</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>R$ 2.390.265,69</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
         <is>
           <t>R$ 3.835.922,27</t>
         </is>
       </c>
-      <c r="F9" t="inlineStr">
-        <is>
-          <t>60,01 %</t>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>62,31 %</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática dos dados: Tue Jan 20 09:38:08 UTC 2026
</commit_message>
<xml_diff>
--- a/dados_dashboard.xlsx
+++ b/dados_dashboard.xlsx
@@ -525,7 +525,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>R$ 382.437,86</t>
+          <t>R$ 419.138,96</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -535,12 +535,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>R$ 382.437,86</t>
+          <t>R$ 419.138,96</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>R$ 382.437,86</t>
+          <t>R$ 419.138,96</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -557,7 +557,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>R$ 321.941,21</t>
+          <t>R$ 399.858,72</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -567,7 +567,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>R$ 321.941,21</t>
+          <t>R$ 399.858,72</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -577,7 +577,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>44,10 %</t>
+          <t>54,78 %</t>
         </is>
       </c>
     </row>
@@ -589,7 +589,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>R$ 286.256,71</t>
+          <t>R$ 289.559,50</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -599,7 +599,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>R$ 286.256,71</t>
+          <t>R$ 289.559,50</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -609,7 +609,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>28.625.671,00 %</t>
+          <t>28.955.950,00 %</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>R$ 236.618,39</t>
+          <t>R$ 271.490,35</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -631,12 +631,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>R$ 236.618,39</t>
+          <t>R$ 271.490,35</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>R$ 236.618,39</t>
+          <t>R$ 271.490,35</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -680,128 +680,128 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>REFUGO MP+CP*</t>
+          <t>MANUTENCAO</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>R$ 141.770,66</t>
+          <t>R$ 179.839,62</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>R$ 0,00</t>
+          <t>R$ 276.953,04</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>R$ 141.770,66</t>
+          <t>R$ 456.792,66</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>R$ 285.000,00</t>
+          <t>R$ 480.000,00</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>49,74 %</t>
+          <t>95,17 %</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MANUTENCAO</t>
+          <t>REFUGO MP+CP*</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>R$ 125.498,86</t>
+          <t>R$ 159.821,42</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>R$ 269.255,54</t>
+          <t>R$ 0,00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>R$ 394.754,40</t>
+          <t>R$ 159.821,42</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>R$ 480.000,00</t>
+          <t>R$ 285.000,00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>82,24 %</t>
+          <t>56,08 %</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>OLEOS E LUBRIFICANTES</t>
+          <t>CUSTO DESENVOLVIMENTO</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>R$ 82.091,98</t>
+          <t>R$ 148.010,88</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>R$ 108.592,70</t>
+          <t>R$ 0,00</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>R$ 190.684,68</t>
+          <t>R$ 148.010,88</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>R$ 280.000,00</t>
+          <t>R$ 148.010,88</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>68,10 %</t>
+          <t>100,00 %</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>CUSTO DESENVOLVIMENTO</t>
+          <t>OLEOS E LUBRIFICANTES</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>R$ 68.563,94</t>
+          <t>R$ 82.091,98</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>R$ 0,00</t>
+          <t>R$ 109.354,76</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>R$ 68.563,94</t>
+          <t>R$ 191.446,74</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>R$ 68.563,94</t>
+          <t>R$ 280.000,00</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>100,00 %</t>
+          <t>68,37 %</t>
         </is>
       </c>
     </row>
@@ -813,17 +813,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>R$ 56.748,18</t>
+          <t>R$ 57.567,20</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>R$ 102.917,80</t>
+          <t>R$ 103.938,96</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>R$ 159.665,98</t>
+          <t>R$ 161.506,16</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -833,7 +833,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>33,97 %</t>
+          <t>34,36 %</t>
         </is>
       </c>
     </row>
@@ -850,12 +850,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>R$ 52.522,04</t>
+          <t>R$ 64.920,59</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>R$ 100.496,12</t>
+          <t>R$ 112.894,67</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -865,7 +865,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>62,81 %</t>
+          <t>70,56 %</t>
         </is>
       </c>
     </row>
@@ -904,12 +904,12 @@
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>CUSTO COM DESENVOLVIMENTO</t>
+          <t>FERRAMENTARIA/MAN FR</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>R$ 8.301,08</t>
+          <t>R$ 8.619,54</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -919,29 +919,29 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>R$ 8.301,08</t>
+          <t>R$ 8.619,54</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>R$ 8.301,08</t>
+          <t>R$ 35.000,00</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>100,00 %</t>
+          <t>24,63 %</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>FERRAMENTARIA/MAN FR</t>
+          <t>CUSTO COM DESENVOLVIMENTO</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>R$ 7.268,32</t>
+          <t>R$ 8.301,08</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -951,17 +951,17 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>R$ 7.268,32</t>
+          <t>R$ 8.301,08</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>R$ 35.000,00</t>
+          <t>R$ 8.301,08</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>20,77 %</t>
+          <t>100,00 %</t>
         </is>
       </c>
     </row>
@@ -1037,27 +1037,27 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>R$ 1.852.943,80</t>
+          <t>R$ 2.141.695,10</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>R$ 537.321,89</t>
+          <t>R$ 559.201,15</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>R$ 2.390.265,69</t>
+          <t>R$ 2.700.896,26</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>R$ 3.835.922,27</t>
+          <t>R$ 3.986.942,27</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>62,31 %</t>
+          <t>67,74 %</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática dos dados: Wed Jan 21 09:38:00 UTC 2026
</commit_message>
<xml_diff>
--- a/dados_dashboard.xlsx
+++ b/dados_dashboard.xlsx
@@ -520,12 +520,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>DEVOLUÃÃO</t>
+          <t>FERRAMENTAS/ MATRIZARIA</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>R$ 419.138,96</t>
+          <t>R$ 447.144,85</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -535,29 +535,29 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>R$ 419.138,96</t>
+          <t>R$ 447.144,85</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>R$ 419.138,96</t>
+          <t>R$ 680.000,00</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>100,00 %</t>
+          <t>65,76 %</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>FERRAMENTAS/ MATRIZARIA</t>
+          <t>DEVOLUÃÃO</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>R$ 399.858,72</t>
+          <t>R$ 438.602,92</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -567,17 +567,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>R$ 399.858,72</t>
+          <t>R$ 438.602,92</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>R$ 730.000,00</t>
+          <t>R$ 438.602,92</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>54,78 %</t>
+          <t>100,00 %</t>
         </is>
       </c>
     </row>
@@ -589,7 +589,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>R$ 289.559,50</t>
+          <t>R$ 368.181,47</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -599,7 +599,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>R$ 289.559,50</t>
+          <t>R$ 368.181,47</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -609,7 +609,7 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>28.955.950,00 %</t>
+          <t>36.818.147,00 %</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>R$ 271.490,35</t>
+          <t>R$ 283.784,61</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -631,12 +631,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>R$ 271.490,35</t>
+          <t>R$ 283.784,61</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>R$ 271.490,35</t>
+          <t>R$ 283.784,61</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -648,64 +648,64 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>FRETES</t>
+          <t>MANUTENCAO</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>R$ 185.370,49</t>
+          <t>R$ 205.025,51</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>R$ 0,00</t>
+          <t>R$ 253.396,69</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>R$ 185.370,49</t>
+          <t>R$ 458.422,20</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>R$ 376.000,00</t>
+          <t>R$ 480.000,00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>49,30 %</t>
+          <t>95,50 %</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MANUTENCAO</t>
+          <t>FRETES</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>R$ 179.839,62</t>
+          <t>R$ 185.370,49</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>R$ 276.953,04</t>
+          <t>R$ 0,00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>R$ 456.792,66</t>
+          <t>R$ 185.370,49</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>R$ 480.000,00</t>
+          <t>R$ 376.000,00</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>95,17 %</t>
+          <t>49,30 %</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>R$ 159.821,42</t>
+          <t>R$ 166.448,51</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -727,17 +727,17 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>R$ 159.821,42</t>
+          <t>R$ 166.448,51</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>R$ 285.000,00</t>
+          <t>R$ 280.000,00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>56,08 %</t>
+          <t>59,45 %</t>
         </is>
       </c>
     </row>
@@ -749,7 +749,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>R$ 148.010,88</t>
+          <t>R$ 154.317,23</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -759,12 +759,12 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>R$ 148.010,88</t>
+          <t>R$ 154.317,23</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>R$ 148.010,88</t>
+          <t>R$ 154.317,23</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
@@ -786,12 +786,12 @@
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>R$ 109.354,76</t>
+          <t>R$ 108.767,66</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>R$ 191.446,74</t>
+          <t>R$ 190.859,64</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -801,7 +801,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>68,37 %</t>
+          <t>68,16 %</t>
         </is>
       </c>
     </row>
@@ -813,27 +813,27 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>R$ 57.567,20</t>
+          <t>R$ 59.268,75</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>R$ 103.938,96</t>
+          <t>R$ 104.851,11</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>R$ 161.506,16</t>
+          <t>R$ 164.119,86</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>R$ 470.000,00</t>
+          <t>R$ 450.000,00</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>34,36 %</t>
+          <t>36,47 %</t>
         </is>
       </c>
     </row>
@@ -850,12 +850,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>R$ 64.920,59</t>
+          <t>R$ 72.265,01</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>R$ 112.894,67</t>
+          <t>R$ 120.239,09</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -865,7 +865,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>70,56 %</t>
+          <t>75,15 %</t>
         </is>
       </c>
     </row>
@@ -978,12 +978,12 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>R$ 4.033,80</t>
+          <t>R$ 4.532,77</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>R$ 4.144,17</t>
+          <t>R$ 4.643,14</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
@@ -993,7 +993,7 @@
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>9,21 %</t>
+          <t>10,32 %</t>
         </is>
       </c>
     </row>
@@ -1037,27 +1037,27 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>R$ 2.141.695,10</t>
+          <t>R$ 2.332.555,21</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>R$ 559.201,15</t>
+          <t>R$ 543.813,25</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>R$ 2.700.896,26</t>
+          <t>R$ 2.876.368,46</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>R$ 3.986.942,27</t>
+          <t>R$ 3.955.006,84</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>67,74 %</t>
+          <t>72,73 %</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática dos dados: Wed Jan 21 23:27:24 UTC 2026
</commit_message>
<xml_diff>
--- a/dados_dashboard.xlsx
+++ b/dados_dashboard.xlsx
@@ -520,12 +520,12 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>FERRAMENTAS/ MATRIZARIA</t>
+          <t>DEVOLUÃÃO</t>
         </is>
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>R$ 447.144,85</t>
+          <t>R$ 653.089,99</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -535,29 +535,29 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>R$ 447.144,85</t>
+          <t>R$ 653.089,99</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>R$ 680.000,00</t>
+          <t>R$ 653.089,99</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
         <is>
-          <t>65,76 %</t>
+          <t>100,00 %</t>
         </is>
       </c>
     </row>
     <row r="3">
       <c r="A3" t="inlineStr">
         <is>
-          <t>DEVOLUÃÃO</t>
+          <t>FERRAMENTAS/ MATRIZARIA</t>
         </is>
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>R$ 438.602,92</t>
+          <t>R$ 471.474,40</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -567,17 +567,17 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>R$ 438.602,92</t>
+          <t>R$ 471.474,40</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>R$ 438.602,92</t>
+          <t>R$ 680.000,00</t>
         </is>
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>100,00 %</t>
+          <t>69,33 %</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>R$ 283.784,61</t>
+          <t>R$ 309.142,60</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -631,12 +631,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>R$ 283.784,61</t>
+          <t>R$ 309.142,60</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>R$ 283.784,61</t>
+          <t>R$ 309.142,60</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -648,76 +648,76 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>MANUTENCAO</t>
+          <t>CUSTO DESENVOLVIMENTO</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>R$ 205.025,51</t>
+          <t>R$ 221.419,59</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>R$ 253.396,69</t>
+          <t>R$ 0,00</t>
         </is>
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>R$ 458.422,20</t>
+          <t>R$ 221.419,59</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>R$ 480.000,00</t>
+          <t>R$ 221.419,59</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>95,50 %</t>
+          <t>100,00 %</t>
         </is>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>FRETES</t>
+          <t>MANUTENCAO</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>R$ 185.370,49</t>
+          <t>R$ 205.025,51</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>R$ 0,00</t>
+          <t>R$ 191.083,29</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>R$ 185.370,49</t>
+          <t>R$ 396.108,80</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>R$ 376.000,00</t>
+          <t>R$ 480.000,00</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>49,30 %</t>
+          <t>82,52 %</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>REFUGO MP+CP*</t>
+          <t>FRETES</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>R$ 166.448,51</t>
+          <t>R$ 185.370,49</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -727,29 +727,29 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>R$ 166.448,51</t>
+          <t>R$ 185.370,49</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>R$ 280.000,00</t>
+          <t>R$ 376.000,00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>59,45 %</t>
+          <t>49,30 %</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>CUSTO DESENVOLVIMENTO</t>
+          <t>REFUGO MP+CP*</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>R$ 154.317,23</t>
+          <t>R$ 184.283,97</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -759,17 +759,17 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>R$ 154.317,23</t>
+          <t>R$ 184.283,97</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>R$ 154.317,23</t>
+          <t>R$ 280.000,00</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>100,00 %</t>
+          <t>65,82 %</t>
         </is>
       </c>
     </row>
@@ -813,17 +813,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>R$ 59.268,75</t>
+          <t>R$ 60.025,93</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>R$ 104.851,11</t>
+          <t>R$ 104.730,86</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>R$ 164.119,86</t>
+          <t>R$ 164.756,79</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -833,7 +833,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>36,47 %</t>
+          <t>36,61 %</t>
         </is>
       </c>
     </row>
@@ -845,7 +845,7 @@
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>R$ 47.974,08</t>
+          <t>R$ 58.564,60</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
@@ -855,7 +855,7 @@
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>R$ 120.239,09</t>
+          <t>R$ 130.829,61</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -865,7 +865,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>75,15 %</t>
+          <t>81,77 %</t>
         </is>
       </c>
     </row>
@@ -909,7 +909,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>R$ 8.619,54</t>
+          <t>R$ 11.114,15</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -919,7 +919,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>R$ 8.619,54</t>
+          <t>R$ 11.114,15</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -929,7 +929,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>24,63 %</t>
+          <t>31,75 %</t>
         </is>
       </c>
     </row>
@@ -1037,27 +1037,27 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>R$ 2.332.555,21</t>
+          <t>R$ 2.677.674,49</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>R$ 543.813,25</t>
+          <t>R$ 481.379,59</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>R$ 2.876.368,46</t>
+          <t>R$ 3.159.054,08</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>R$ 3.955.006,84</t>
+          <t>R$ 4.261.954,26</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>72,73 %</t>
+          <t>74,12 %</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática dos dados: Thu Jan 22 09:38:05 UTC 2026
</commit_message>
<xml_diff>
--- a/dados_dashboard.xlsx
+++ b/dados_dashboard.xlsx
@@ -818,12 +818,12 @@
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>R$ 104.730,86</t>
+          <t>R$ 104.843,84</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>R$ 164.756,79</t>
+          <t>R$ 164.869,77</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -833,7 +833,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>36,61 %</t>
+          <t>36,64 %</t>
         </is>
       </c>
     </row>
@@ -1042,12 +1042,12 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>R$ 481.379,59</t>
+          <t>R$ 481.492,57</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>R$ 3.159.054,08</t>
+          <t>R$ 3.159.167,06</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">

</xml_diff>

<commit_message>
Atualização automática dos dados: Fri Jan 23 09:35:37 UTC 2026
</commit_message>
<xml_diff>
--- a/dados_dashboard.xlsx
+++ b/dados_dashboard.xlsx
@@ -525,7 +525,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>R$ 653.089,99</t>
+          <t>R$ 777.126,11</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -535,12 +535,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>R$ 653.089,99</t>
+          <t>R$ 777.126,11</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>R$ 653.089,99</t>
+          <t>R$ 777.126,11</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -557,7 +557,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>R$ 471.474,40</t>
+          <t>R$ 528.494,31</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -567,7 +567,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>R$ 471.474,40</t>
+          <t>R$ 528.494,31</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -577,7 +577,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>69,33 %</t>
+          <t>77,72 %</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>R$ 309.142,60</t>
+          <t>R$ 328.104,17</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -631,12 +631,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>R$ 309.142,60</t>
+          <t>R$ 328.104,17</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>R$ 309.142,60</t>
+          <t>R$ 328.104,17</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -653,7 +653,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>R$ 221.419,59</t>
+          <t>R$ 313.457,68</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -663,12 +663,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>R$ 221.419,59</t>
+          <t>R$ 313.457,68</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>R$ 221.419,59</t>
+          <t>R$ 313.457,68</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -680,64 +680,64 @@
     <row r="7">
       <c r="A7" t="inlineStr">
         <is>
-          <t>MANUTENCAO</t>
+          <t>FRETES</t>
         </is>
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>R$ 205.025,51</t>
+          <t>R$ 214.614,62</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>R$ 191.083,29</t>
+          <t>R$ 0,00</t>
         </is>
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>R$ 396.108,80</t>
+          <t>R$ 214.614,62</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>R$ 480.000,00</t>
+          <t>R$ 376.000,00</t>
         </is>
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>82,52 %</t>
+          <t>57,08 %</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>FRETES</t>
+          <t>MANUTENCAO</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>R$ 185.370,49</t>
+          <t>R$ 206.862,29</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>R$ 0,00</t>
+          <t>R$ 191.636,71</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>R$ 185.370,49</t>
+          <t>R$ 398.499,00</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>R$ 376.000,00</t>
+          <t>R$ 480.000,00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>49,30 %</t>
+          <t>83,02 %</t>
         </is>
       </c>
     </row>
@@ -749,7 +749,7 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>R$ 184.283,97</t>
+          <t>R$ 195.167,49</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
@@ -759,7 +759,7 @@
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>R$ 184.283,97</t>
+          <t>R$ 195.167,49</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -769,71 +769,71 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>65,82 %</t>
+          <t>69,70 %</t>
         </is>
       </c>
     </row>
     <row r="10">
       <c r="A10" t="inlineStr">
         <is>
-          <t>OLEOS E LUBRIFICANTES</t>
+          <t>DESP. INDUSTRIAL</t>
         </is>
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>R$ 82.091,98</t>
+          <t>R$ 187.496,71</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>R$ 108.767,66</t>
+          <t>R$ 109.131,35</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>R$ 190.859,64</t>
+          <t>R$ 296.628,06</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
         <is>
-          <t>R$ 280.000,00</t>
+          <t>R$ 450.000,00</t>
         </is>
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>68,16 %</t>
+          <t>65,92 %</t>
         </is>
       </c>
     </row>
     <row r="11">
       <c r="A11" t="inlineStr">
         <is>
-          <t>DESP. INDUSTRIAL</t>
+          <t>OLEOS E LUBRIFICANTES</t>
         </is>
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>R$ 60.025,93</t>
+          <t>R$ 82.091,98</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>R$ 104.843,84</t>
+          <t>R$ 108.767,66</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>R$ 164.869,77</t>
+          <t>R$ 190.859,64</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
         <is>
-          <t>R$ 450.000,00</t>
+          <t>R$ 280.000,00</t>
         </is>
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>36,64 %</t>
+          <t>68,16 %</t>
         </is>
       </c>
     </row>
@@ -850,12 +850,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>R$ 72.265,01</t>
+          <t>R$ 97.082,75</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>R$ 130.829,61</t>
+          <t>R$ 155.647,35</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -865,7 +865,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>81,77 %</t>
+          <t>97,28 %</t>
         </is>
       </c>
     </row>
@@ -941,7 +941,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>R$ 8.301,08</t>
+          <t>R$ 8.615,99</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -951,12 +951,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>R$ 8.301,08</t>
+          <t>R$ 8.615,99</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>R$ 8.301,08</t>
+          <t>R$ 8.615,99</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1037,27 +1037,27 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>R$ 2.677.674,49</t>
+          <t>R$ 3.128.596,78</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>R$ 481.492,57</t>
+          <t>R$ 511.151,23</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>R$ 3.159.167,06</t>
+          <t>R$ 3.639.748,01</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>R$ 4.261.954,26</t>
+          <t>R$ 4.497.304,95</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>74,12 %</t>
+          <t>80,93 %</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática dos dados: Mon Jan 26 09:39:43 UTC 2026
</commit_message>
<xml_diff>
--- a/dados_dashboard.xlsx
+++ b/dados_dashboard.xlsx
@@ -557,7 +557,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>R$ 528.494,31</t>
+          <t>R$ 541.715,15</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -567,7 +567,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>R$ 528.494,31</t>
+          <t>R$ 541.715,15</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -577,7 +577,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>77,72 %</t>
+          <t>79,66 %</t>
         </is>
       </c>
     </row>
@@ -589,7 +589,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>R$ 368.181,47</t>
+          <t>R$ 371.686,93</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -599,7 +599,7 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>R$ 368.181,47</t>
+          <t>R$ 371.686,93</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
@@ -609,19 +609,19 @@
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>36.818.147,00 %</t>
+          <t>37.168.693,00 %</t>
         </is>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="inlineStr">
         <is>
-          <t>REFUGO REAL (PROCESSO)</t>
+          <t>CUSTO DESENVOLVIMENTO</t>
         </is>
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>R$ 328.104,17</t>
+          <t>R$ 370.293,54</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -631,12 +631,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>R$ 328.104,17</t>
+          <t>R$ 370.293,54</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>R$ 328.104,17</t>
+          <t>R$ 370.293,54</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -648,12 +648,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>CUSTO DESENVOLVIMENTO</t>
+          <t>REFUGO REAL (PROCESSO)</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>R$ 313.457,68</t>
+          <t>R$ 357.461,99</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -663,12 +663,12 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>R$ 313.457,68</t>
+          <t>R$ 357.461,99</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>R$ 313.457,68</t>
+          <t>R$ 357.461,99</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
@@ -685,7 +685,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>R$ 214.614,62</t>
+          <t>R$ 258.961,64</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -695,7 +695,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>R$ 214.614,62</t>
+          <t>R$ 258.961,64</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -705,71 +705,71 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>57,08 %</t>
+          <t>68,87 %</t>
         </is>
       </c>
     </row>
     <row r="8">
       <c r="A8" t="inlineStr">
         <is>
-          <t>MANUTENCAO</t>
+          <t>REFUGO MP+CP*</t>
         </is>
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>R$ 206.862,29</t>
+          <t>R$ 212.131,03</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>R$ 191.636,71</t>
+          <t>R$ 0,00</t>
         </is>
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>R$ 398.499,00</t>
+          <t>R$ 212.131,03</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
         <is>
-          <t>R$ 480.000,00</t>
+          <t>R$ 280.000,00</t>
         </is>
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>83,02 %</t>
+          <t>75,76 %</t>
         </is>
       </c>
     </row>
     <row r="9">
       <c r="A9" t="inlineStr">
         <is>
-          <t>REFUGO MP+CP*</t>
+          <t>MANUTENCAO</t>
         </is>
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>R$ 195.167,49</t>
+          <t>R$ 209.640,19</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>R$ 0,00</t>
+          <t>R$ 192.005,09</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>R$ 195.167,49</t>
+          <t>R$ 401.645,28</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
         <is>
-          <t>R$ 280.000,00</t>
+          <t>R$ 480.000,00</t>
         </is>
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>69,70 %</t>
+          <t>83,68 %</t>
         </is>
       </c>
     </row>
@@ -781,17 +781,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>R$ 187.496,71</t>
+          <t>R$ 168.751,13</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>R$ 109.131,35</t>
+          <t>R$ 121.898,00</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>R$ 296.628,06</t>
+          <t>R$ 290.649,13</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -801,7 +801,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>65,92 %</t>
+          <t>64,59 %</t>
         </is>
       </c>
     </row>
@@ -813,7 +813,7 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>R$ 82.091,98</t>
+          <t>R$ 110.014,09</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
@@ -823,7 +823,7 @@
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>R$ 190.859,64</t>
+          <t>R$ 218.781,75</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -833,7 +833,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>68,16 %</t>
+          <t>78,14 %</t>
         </is>
       </c>
     </row>
@@ -850,12 +850,12 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>R$ 97.082,75</t>
+          <t>R$ 74.942,31</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>R$ 155.647,35</t>
+          <t>R$ 133.506,91</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
@@ -865,7 +865,7 @@
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>97,28 %</t>
+          <t>83,44 %</t>
         </is>
       </c>
     </row>
@@ -877,7 +877,7 @@
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>R$ 43.762,33</t>
+          <t>R$ 49.915,98</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
@@ -887,7 +887,7 @@
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>R$ 43.762,33</t>
+          <t>R$ 49.915,98</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -897,7 +897,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>97,25 %</t>
+          <t>110,92 %</t>
         </is>
       </c>
     </row>
@@ -909,7 +909,7 @@
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>R$ 11.114,15</t>
+          <t>R$ 11.273,87</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -919,7 +919,7 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>R$ 11.114,15</t>
+          <t>R$ 11.273,87</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
@@ -929,7 +929,7 @@
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>31,75 %</t>
+          <t>32,21 %</t>
         </is>
       </c>
     </row>
@@ -941,7 +941,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>R$ 8.615,99</t>
+          <t>R$ 9.192,99</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -951,12 +951,12 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>R$ 8.615,99</t>
+          <t>R$ 9.192,99</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>R$ 8.615,99</t>
+          <t>R$ 9.192,99</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
@@ -1037,27 +1037,27 @@
       </c>
       <c r="B18" t="inlineStr">
         <is>
-          <t>R$ 3.128.596,78</t>
+          <t>R$ 3.294.708,58</t>
         </is>
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>R$ 511.151,23</t>
+          <t>R$ 502.145,83</t>
         </is>
       </c>
       <c r="D18" t="inlineStr">
         <is>
-          <t>R$ 3.639.748,01</t>
+          <t>R$ 3.796.854,41</t>
         </is>
       </c>
       <c r="E18" t="inlineStr">
         <is>
-          <t>R$ 4.497.304,95</t>
+          <t>R$ 4.584.075,63</t>
         </is>
       </c>
       <c r="F18" t="inlineStr">
         <is>
-          <t>80,93 %</t>
+          <t>82,83 %</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática dos dados: Tue Jan 27 09:38:30 UTC 2026
</commit_message>
<xml_diff>
--- a/dados_dashboard.xlsx
+++ b/dados_dashboard.xlsx
@@ -477,7 +477,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:F18"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -525,7 +525,7 @@
       </c>
       <c r="B2" t="inlineStr">
         <is>
-          <t>R$ 777.126,11</t>
+          <t>R$ 777.651,96</t>
         </is>
       </c>
       <c r="C2" t="inlineStr">
@@ -535,12 +535,12 @@
       </c>
       <c r="D2" t="inlineStr">
         <is>
-          <t>R$ 777.126,11</t>
+          <t>R$ 777.651,96</t>
         </is>
       </c>
       <c r="E2" t="inlineStr">
         <is>
-          <t>R$ 777.126,11</t>
+          <t>R$ 777.651,96</t>
         </is>
       </c>
       <c r="F2" t="inlineStr">
@@ -557,7 +557,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>R$ 541.715,15</t>
+          <t>R$ 566.678,29</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -567,7 +567,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>R$ 541.715,15</t>
+          <t>R$ 566.678,29</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -577,19 +577,19 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>79,66 %</t>
+          <t>83,34 %</t>
         </is>
       </c>
     </row>
     <row r="4">
       <c r="A4" t="inlineStr">
         <is>
-          <t>MATERIA PRIMA</t>
+          <t>REFUGO REAL (PROCESSO)</t>
         </is>
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>R$ 371.686,93</t>
+          <t>R$ 388.596,40</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -599,17 +599,17 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>R$ 371.686,93</t>
+          <t>R$ 388.596,40</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>R$ 1,00</t>
+          <t>R$ 388.596,40</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
         <is>
-          <t>37.168.693,00 %</t>
+          <t>100,00 %</t>
         </is>
       </c>
     </row>
@@ -621,7 +621,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>R$ 370.293,54</t>
+          <t>R$ 371.996,61</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -631,12 +631,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>R$ 370.293,54</t>
+          <t>R$ 371.996,61</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>R$ 370.293,54</t>
+          <t>R$ 371.996,61</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -648,12 +648,12 @@
     <row r="6">
       <c r="A6" t="inlineStr">
         <is>
-          <t>REFUGO REAL (PROCESSO)</t>
+          <t>MATERIA PRIMA</t>
         </is>
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>R$ 357.461,99</t>
+          <t>R$ 371.686,93</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -663,17 +663,17 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>R$ 357.461,99</t>
+          <t>R$ 371.686,93</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
         <is>
-          <t>R$ 357.461,99</t>
+          <t>R$ 1,00</t>
         </is>
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>100,00 %</t>
+          <t>37.168.693,00 %</t>
         </is>
       </c>
     </row>
@@ -685,7 +685,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>R$ 258.961,64</t>
+          <t>R$ 264.055,72</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -695,7 +695,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>R$ 258.961,64</t>
+          <t>R$ 264.055,72</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -705,7 +705,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>68,87 %</t>
+          <t>70,23 %</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>R$ 212.131,03</t>
+          <t>R$ 233.797,08</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -727,7 +727,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>R$ 212.131,03</t>
+          <t>R$ 233.797,08</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -737,7 +737,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>75,76 %</t>
+          <t>83,50 %</t>
         </is>
       </c>
     </row>
@@ -749,17 +749,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>R$ 209.640,19</t>
+          <t>R$ 210.332,87</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>R$ 192.005,09</t>
+          <t>R$ 192.360,13</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>R$ 401.645,28</t>
+          <t>R$ 402.693,00</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -769,7 +769,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>83,68 %</t>
+          <t>83,89 %</t>
         </is>
       </c>
     </row>
@@ -781,17 +781,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>R$ 168.751,13</t>
+          <t>R$ 204.850,27</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>R$ 121.898,00</t>
+          <t>R$ 126.956,46</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>R$ 290.649,13</t>
+          <t>R$ 331.806,73</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -801,7 +801,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>64,59 %</t>
+          <t>73,73 %</t>
         </is>
       </c>
     </row>
@@ -840,76 +840,76 @@
     <row r="12">
       <c r="A12" t="inlineStr">
         <is>
-          <t>EMBALAGENS</t>
+          <t>DÃBITOS QUALIDADE</t>
         </is>
       </c>
       <c r="B12" t="inlineStr">
         <is>
-          <t>R$ 58.564,60</t>
+          <t>R$ 93.736,50</t>
         </is>
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>R$ 74.942,31</t>
+          <t>R$ 0,00</t>
         </is>
       </c>
       <c r="D12" t="inlineStr">
         <is>
-          <t>R$ 133.506,91</t>
+          <t>R$ 93.736,50</t>
         </is>
       </c>
       <c r="E12" t="inlineStr">
         <is>
-          <t>R$ 160.000,00</t>
+          <t>R$ 93.736,50</t>
         </is>
       </c>
       <c r="F12" t="inlineStr">
         <is>
-          <t>83,44 %</t>
+          <t>100,00 %</t>
         </is>
       </c>
     </row>
     <row r="13">
       <c r="A13" t="inlineStr">
         <is>
-          <t>SERVICOS DE QUALIDADE</t>
+          <t>EMBALAGENS</t>
         </is>
       </c>
       <c r="B13" t="inlineStr">
         <is>
-          <t>R$ 49.915,98</t>
+          <t>R$ 58.564,60</t>
         </is>
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>R$ 0,00</t>
+          <t>R$ 80.342,89</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>R$ 49.915,98</t>
+          <t>R$ 138.907,49</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
         <is>
-          <t>R$ 45.000,00</t>
+          <t>R$ 160.000,00</t>
         </is>
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>110,92 %</t>
+          <t>86,82 %</t>
         </is>
       </c>
     </row>
     <row r="14">
       <c r="A14" t="inlineStr">
         <is>
-          <t>FERRAMENTARIA/MAN FR</t>
+          <t>SERVICOS DE QUALIDADE</t>
         </is>
       </c>
       <c r="B14" t="inlineStr">
         <is>
-          <t>R$ 11.273,87</t>
+          <t>R$ 49.915,98</t>
         </is>
       </c>
       <c r="C14" t="inlineStr">
@@ -919,29 +919,29 @@
       </c>
       <c r="D14" t="inlineStr">
         <is>
-          <t>R$ 11.273,87</t>
+          <t>R$ 49.915,98</t>
         </is>
       </c>
       <c r="E14" t="inlineStr">
         <is>
-          <t>R$ 35.000,00</t>
+          <t>R$ 45.000,00</t>
         </is>
       </c>
       <c r="F14" t="inlineStr">
         <is>
-          <t>32,21 %</t>
+          <t>110,92 %</t>
         </is>
       </c>
     </row>
     <row r="15">
       <c r="A15" t="inlineStr">
         <is>
-          <t>CUSTO COM DESENVOLVIMENTO</t>
+          <t>FERRAMENTARIA/MAN FR</t>
         </is>
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>R$ 9.192,99</t>
+          <t>R$ 12.218,35</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -951,113 +951,145 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>R$ 9.192,99</t>
+          <t>R$ 12.218,35</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
         <is>
-          <t>R$ 9.192,99</t>
+          <t>R$ 35.000,00</t>
         </is>
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>100,00 %</t>
+          <t>34,91 %</t>
         </is>
       </c>
     </row>
     <row r="16">
       <c r="A16" t="inlineStr">
         <is>
-          <t>MATERIAL QUALIDADE</t>
+          <t>CUSTO COM DESENVOLVIMENTO</t>
         </is>
       </c>
       <c r="B16" t="inlineStr">
         <is>
-          <t>R$ 110,37</t>
+          <t>R$ 9.192,99</t>
         </is>
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>R$ 4.532,77</t>
+          <t>R$ 0,00</t>
         </is>
       </c>
       <c r="D16" t="inlineStr">
         <is>
-          <t>R$ 4.643,14</t>
+          <t>R$ 9.192,99</t>
         </is>
       </c>
       <c r="E16" t="inlineStr">
         <is>
-          <t>R$ 45.000,00</t>
+          <t>R$ 9.192,99</t>
         </is>
       </c>
       <c r="F16" t="inlineStr">
         <is>
-          <t>10,32 %</t>
+          <t>100,00 %</t>
         </is>
       </c>
     </row>
     <row r="17">
       <c r="A17" t="inlineStr">
         <is>
-          <t>ENERGIA ELETRICA</t>
+          <t>MATERIAL QUALIDADE</t>
         </is>
       </c>
       <c r="B17" t="inlineStr">
         <is>
-          <t>R$ 0,00</t>
+          <t>R$ 4.474,35</t>
         </is>
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>R$ 0,00</t>
+          <t>R$ 4.532,77</t>
         </is>
       </c>
       <c r="D17" t="inlineStr">
         <is>
-          <t>R$ 0,00</t>
+          <t>R$ 9.007,12</t>
         </is>
       </c>
       <c r="E17" t="inlineStr">
         <is>
-          <t>R$ 519.000,00</t>
+          <t>R$ 45.000,00</t>
         </is>
       </c>
       <c r="F17" t="inlineStr">
         <is>
-          <t>0 %</t>
+          <t>20,02 %</t>
         </is>
       </c>
     </row>
     <row r="18">
       <c r="A18" t="inlineStr">
         <is>
+          <t>ENERGIA ELETRICA</t>
+        </is>
+      </c>
+      <c r="B18" t="inlineStr">
+        <is>
+          <t>R$ 0,00</t>
+        </is>
+      </c>
+      <c r="C18" t="inlineStr">
+        <is>
+          <t>R$ 0,00</t>
+        </is>
+      </c>
+      <c r="D18" t="inlineStr">
+        <is>
+          <t>R$ 0,00</t>
+        </is>
+      </c>
+      <c r="E18" t="inlineStr">
+        <is>
+          <t>R$ 519.000,00</t>
+        </is>
+      </c>
+      <c r="F18" t="inlineStr">
+        <is>
+          <t>0 %</t>
+        </is>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" t="inlineStr">
+        <is>
           <t>Total Geral</t>
         </is>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>R$ 3.294.708,58</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>R$ 502.145,83</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>R$ 3.796.854,41</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>R$ 4.584.075,63</t>
-        </is>
-      </c>
-      <c r="F18" t="inlineStr">
-        <is>
-          <t>82,83 %</t>
+      <c r="B19" t="inlineStr">
+        <is>
+          <t>R$ 3.493.965,91</t>
+        </is>
+      </c>
+      <c r="C19" t="inlineStr">
+        <is>
+          <t>R$ 512.959,91</t>
+        </is>
+      </c>
+      <c r="D19" t="inlineStr">
+        <is>
+          <t>R$ 4.006.925,82</t>
+        </is>
+      </c>
+      <c r="E19" t="inlineStr">
+        <is>
+          <t>R$ 4.711.175,46</t>
+        </is>
+      </c>
+      <c r="F19" t="inlineStr">
+        <is>
+          <t>85,05 %</t>
         </is>
       </c>
     </row>

</xml_diff>

<commit_message>
Atualização automática dos dados: Wed Jan 28 09:39:19 UTC 2026
</commit_message>
<xml_diff>
--- a/dados_dashboard.xlsx
+++ b/dados_dashboard.xlsx
@@ -557,7 +557,7 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>R$ 566.678,29</t>
+          <t>R$ 576.506,64</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
@@ -567,7 +567,7 @@
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>R$ 566.678,29</t>
+          <t>R$ 576.506,64</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
@@ -577,7 +577,7 @@
       </c>
       <c r="F3" t="inlineStr">
         <is>
-          <t>83,34 %</t>
+          <t>84,78 %</t>
         </is>
       </c>
     </row>
@@ -589,7 +589,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>R$ 388.596,40</t>
+          <t>R$ 412.721,56</t>
         </is>
       </c>
       <c r="C4" t="inlineStr">
@@ -599,12 +599,12 @@
       </c>
       <c r="D4" t="inlineStr">
         <is>
-          <t>R$ 388.596,40</t>
+          <t>R$ 412.721,56</t>
         </is>
       </c>
       <c r="E4" t="inlineStr">
         <is>
-          <t>R$ 388.596,40</t>
+          <t>R$ 412.721,56</t>
         </is>
       </c>
       <c r="F4" t="inlineStr">
@@ -621,7 +621,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>R$ 371.996,61</t>
+          <t>R$ 404.800,85</t>
         </is>
       </c>
       <c r="C5" t="inlineStr">
@@ -631,12 +631,12 @@
       </c>
       <c r="D5" t="inlineStr">
         <is>
-          <t>R$ 371.996,61</t>
+          <t>R$ 404.800,85</t>
         </is>
       </c>
       <c r="E5" t="inlineStr">
         <is>
-          <t>R$ 371.996,61</t>
+          <t>R$ 404.800,85</t>
         </is>
       </c>
       <c r="F5" t="inlineStr">
@@ -653,7 +653,7 @@
       </c>
       <c r="B6" t="inlineStr">
         <is>
-          <t>R$ 371.686,93</t>
+          <t>R$ 376.822,93</t>
         </is>
       </c>
       <c r="C6" t="inlineStr">
@@ -663,7 +663,7 @@
       </c>
       <c r="D6" t="inlineStr">
         <is>
-          <t>R$ 371.686,93</t>
+          <t>R$ 376.822,93</t>
         </is>
       </c>
       <c r="E6" t="inlineStr">
@@ -673,7 +673,7 @@
       </c>
       <c r="F6" t="inlineStr">
         <is>
-          <t>37.168.693,00 %</t>
+          <t>37.682.293,00 %</t>
         </is>
       </c>
     </row>
@@ -685,7 +685,7 @@
       </c>
       <c r="B7" t="inlineStr">
         <is>
-          <t>R$ 264.055,72</t>
+          <t>R$ 275.933,53</t>
         </is>
       </c>
       <c r="C7" t="inlineStr">
@@ -695,7 +695,7 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>R$ 264.055,72</t>
+          <t>R$ 275.933,53</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
@@ -705,7 +705,7 @@
       </c>
       <c r="F7" t="inlineStr">
         <is>
-          <t>70,23 %</t>
+          <t>73,39 %</t>
         </is>
       </c>
     </row>
@@ -717,7 +717,7 @@
       </c>
       <c r="B8" t="inlineStr">
         <is>
-          <t>R$ 233.797,08</t>
+          <t>R$ 248.550,01</t>
         </is>
       </c>
       <c r="C8" t="inlineStr">
@@ -727,7 +727,7 @@
       </c>
       <c r="D8" t="inlineStr">
         <is>
-          <t>R$ 233.797,08</t>
+          <t>R$ 248.550,01</t>
         </is>
       </c>
       <c r="E8" t="inlineStr">
@@ -737,7 +737,7 @@
       </c>
       <c r="F8" t="inlineStr">
         <is>
-          <t>83,50 %</t>
+          <t>88,77 %</t>
         </is>
       </c>
     </row>
@@ -749,17 +749,17 @@
       </c>
       <c r="B9" t="inlineStr">
         <is>
-          <t>R$ 210.332,87</t>
+          <t>R$ 215.675,40</t>
         </is>
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>R$ 192.360,13</t>
+          <t>R$ 192.974,77</t>
         </is>
       </c>
       <c r="D9" t="inlineStr">
         <is>
-          <t>R$ 402.693,00</t>
+          <t>R$ 408.650,17</t>
         </is>
       </c>
       <c r="E9" t="inlineStr">
@@ -769,7 +769,7 @@
       </c>
       <c r="F9" t="inlineStr">
         <is>
-          <t>83,89 %</t>
+          <t>85,14 %</t>
         </is>
       </c>
     </row>
@@ -781,17 +781,17 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>R$ 204.850,27</t>
+          <t>R$ 205.846,84</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>R$ 126.956,46</t>
+          <t>R$ 130.664,97</t>
         </is>
       </c>
       <c r="D10" t="inlineStr">
         <is>
-          <t>R$ 331.806,73</t>
+          <t>R$ 336.511,81</t>
         </is>
       </c>
       <c r="E10" t="inlineStr">
@@ -801,7 +801,7 @@
       </c>
       <c r="F10" t="inlineStr">
         <is>
-          <t>73,73 %</t>
+          <t>74,78 %</t>
         </is>
       </c>
     </row>
@@ -813,17 +813,17 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>R$ 110.014,09</t>
+          <t>R$ 110.944,71</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>R$ 108.767,66</t>
+          <t>R$ 108.806,99</t>
         </is>
       </c>
       <c r="D11" t="inlineStr">
         <is>
-          <t>R$ 218.781,75</t>
+          <t>R$ 219.751,70</t>
         </is>
       </c>
       <c r="E11" t="inlineStr">
@@ -833,7 +833,7 @@
       </c>
       <c r="F11" t="inlineStr">
         <is>
-          <t>78,14 %</t>
+          <t>78,48 %</t>
         </is>
       </c>
     </row>
@@ -882,12 +882,12 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>R$ 80.342,89</t>
+          <t>R$ 82.468,43</t>
         </is>
       </c>
       <c r="D13" t="inlineStr">
         <is>
-          <t>R$ 138.907,49</t>
+          <t>R$ 141.033,03</t>
         </is>
       </c>
       <c r="E13" t="inlineStr">
@@ -897,7 +897,7 @@
       </c>
       <c r="F13" t="inlineStr">
         <is>
-          <t>86,82 %</t>
+          <t>88,15 %</t>
         </is>
       </c>
     </row>
@@ -941,7 +941,7 @@
       </c>
       <c r="B15" t="inlineStr">
         <is>
-          <t>R$ 12.218,35</t>
+          <t>R$ 12.427,98</t>
         </is>
       </c>
       <c r="C15" t="inlineStr">
@@ -951,7 +951,7 @@
       </c>
       <c r="D15" t="inlineStr">
         <is>
-          <t>R$ 12.218,35</t>
+          <t>R$ 12.427,98</t>
         </is>
       </c>
       <c r="E15" t="inlineStr">
@@ -961,7 +961,7 @@
       </c>
       <c r="F15" t="inlineStr">
         <is>
-          <t>34,91 %</t>
+          <t>35,51 %</t>
         </is>
       </c>
     </row>
@@ -1069,27 +1069,27 @@
       </c>
       <c r="B19" t="inlineStr">
         <is>
-          <t>R$ 3.493.965,91</t>
+          <t>R$ 3.585.216,82</t>
         </is>
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>R$ 512.959,91</t>
+          <t>R$ 519.447,93</t>
         </is>
       </c>
       <c r="D19" t="inlineStr">
         <is>
-          <t>R$ 4.006.925,82</t>
+          <t>R$ 4.104.664,75</t>
         </is>
       </c>
       <c r="E19" t="inlineStr">
         <is>
-          <t>R$ 4.711.175,46</t>
+          <t>R$ 4.768.104,86</t>
         </is>
       </c>
       <c r="F19" t="inlineStr">
         <is>
-          <t>85,05 %</t>
+          <t>86,09 %</t>
         </is>
       </c>
     </row>

</xml_diff>